<commit_message>
fixed toxgreen dataset; combined G9 and G10
</commit_message>
<xml_diff>
--- a/2023-9-8_oligoPoolOrder/2023-11-4_TOXGREEN_analyzed.xlsx
+++ b/2023-9-8_oligoPoolOrder/2023-11-4_TOXGREEN_analyzed.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26924"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27231"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\github\Sequence-Design\2023-9-8_oligoPoolOrder\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E5BA2E2D-CAAB-423F-948D-FEF98AA100F4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F95188BE-5F92-44B7-8996-2842FF084261}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="45972" yWindow="3636" windowWidth="30936" windowHeight="16776" xr2:uid="{5945CEB6-EA6B-4443-91CF-E588C23E1956}"/>
+    <workbookView xWindow="45984" yWindow="3744" windowWidth="15552" windowHeight="16656" xr2:uid="{5945CEB6-EA6B-4443-91CF-E588C23E1956}"/>
   </bookViews>
   <sheets>
     <sheet name="top" sheetId="1" r:id="rId1"/>
@@ -231,7 +231,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="406" uniqueCount="163">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="408" uniqueCount="165">
   <si>
     <t>Application: Tecan i-control</t>
   </si>
@@ -721,6 +721,12 @@
   <si>
     <t>Standard Deviation</t>
   </si>
+  <si>
+    <t>G9+G10 (same sequence)</t>
+  </si>
+  <si>
+    <t>G9+G10</t>
+  </si>
 </sst>
 </file>
 
@@ -1115,10 +1121,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4E908059-E272-4A56-8E65-E3ED9D3BF650}">
-  <dimension ref="A1:AZ183"/>
+  <dimension ref="A1:AZ184"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A145" workbookViewId="0">
-      <selection activeCell="O170" sqref="O170"/>
+    <sheetView tabSelected="1" topLeftCell="A148" workbookViewId="0">
+      <selection activeCell="H184" sqref="H184:L184"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -17142,6 +17148,215 @@
         <v>13779</v>
       </c>
     </row>
+    <row r="159" spans="1:52" x14ac:dyDescent="0.4">
+      <c r="A159" s="3" t="s">
+        <v>163</v>
+      </c>
+      <c r="B159">
+        <f>AVERAGE(B124,B131,B115,B70,B110,B92)</f>
+        <v>20542.166666666668</v>
+      </c>
+      <c r="C159">
+        <f t="shared" ref="C159:AZ159" si="22">AVERAGE(C124,C131,C115,C70,C110,C92)</f>
+        <v>24325</v>
+      </c>
+      <c r="D159">
+        <f t="shared" si="22"/>
+        <v>27167</v>
+      </c>
+      <c r="E159">
+        <f t="shared" si="22"/>
+        <v>30339</v>
+      </c>
+      <c r="F159">
+        <f t="shared" si="22"/>
+        <v>33040.5</v>
+      </c>
+      <c r="G159">
+        <f t="shared" si="22"/>
+        <v>35054.166666666664</v>
+      </c>
+      <c r="H159">
+        <f t="shared" si="22"/>
+        <v>36897.666666666664</v>
+      </c>
+      <c r="I159">
+        <f t="shared" si="22"/>
+        <v>38102.166666666664</v>
+      </c>
+      <c r="J159">
+        <f t="shared" si="22"/>
+        <v>38738.333333333336</v>
+      </c>
+      <c r="K159">
+        <f t="shared" si="22"/>
+        <v>38728.333333333336</v>
+      </c>
+      <c r="L159">
+        <f t="shared" si="22"/>
+        <v>38757.166666666664</v>
+      </c>
+      <c r="M159">
+        <f t="shared" si="22"/>
+        <v>38427.666666666664</v>
+      </c>
+      <c r="N159">
+        <f t="shared" si="22"/>
+        <v>37892.333333333336</v>
+      </c>
+      <c r="O159">
+        <f t="shared" si="22"/>
+        <v>37576.166666666664</v>
+      </c>
+      <c r="P159">
+        <f t="shared" si="22"/>
+        <v>37065.5</v>
+      </c>
+      <c r="Q159">
+        <f t="shared" si="22"/>
+        <v>36957.333333333336</v>
+      </c>
+      <c r="R159">
+        <f t="shared" si="22"/>
+        <v>36606.333333333336</v>
+      </c>
+      <c r="S159">
+        <f t="shared" si="22"/>
+        <v>36322.333333333336</v>
+      </c>
+      <c r="T159">
+        <f t="shared" si="22"/>
+        <v>36247</v>
+      </c>
+      <c r="U159">
+        <f t="shared" si="22"/>
+        <v>36029</v>
+      </c>
+      <c r="V159">
+        <f t="shared" si="22"/>
+        <v>35485</v>
+      </c>
+      <c r="W159">
+        <f t="shared" si="22"/>
+        <v>35293</v>
+      </c>
+      <c r="X159">
+        <f t="shared" si="22"/>
+        <v>34540.166666666664</v>
+      </c>
+      <c r="Y159">
+        <f t="shared" si="22"/>
+        <v>34243.333333333336</v>
+      </c>
+      <c r="Z159">
+        <f t="shared" si="22"/>
+        <v>33340.166666666664</v>
+      </c>
+      <c r="AA159">
+        <f t="shared" si="22"/>
+        <v>32674</v>
+      </c>
+      <c r="AB159">
+        <f t="shared" si="22"/>
+        <v>32230.666666666668</v>
+      </c>
+      <c r="AC159">
+        <f t="shared" si="22"/>
+        <v>31465.166666666668</v>
+      </c>
+      <c r="AD159">
+        <f t="shared" si="22"/>
+        <v>30684.833333333332</v>
+      </c>
+      <c r="AE159">
+        <f t="shared" si="22"/>
+        <v>30082.833333333332</v>
+      </c>
+      <c r="AF159">
+        <f t="shared" si="22"/>
+        <v>28884.5</v>
+      </c>
+      <c r="AG159">
+        <f t="shared" si="22"/>
+        <v>28425.166666666668</v>
+      </c>
+      <c r="AH159">
+        <f t="shared" si="22"/>
+        <v>27372.333333333332</v>
+      </c>
+      <c r="AI159">
+        <f t="shared" si="22"/>
+        <v>26345.5</v>
+      </c>
+      <c r="AJ159">
+        <f t="shared" si="22"/>
+        <v>25775.833333333332</v>
+      </c>
+      <c r="AK159">
+        <f t="shared" si="22"/>
+        <v>24719.333333333332</v>
+      </c>
+      <c r="AL159">
+        <f t="shared" si="22"/>
+        <v>24114.5</v>
+      </c>
+      <c r="AM159">
+        <f t="shared" si="22"/>
+        <v>23189.5</v>
+      </c>
+      <c r="AN159">
+        <f t="shared" si="22"/>
+        <v>22301.666666666668</v>
+      </c>
+      <c r="AO159">
+        <f t="shared" si="22"/>
+        <v>21739</v>
+      </c>
+      <c r="AP159">
+        <f t="shared" si="22"/>
+        <v>20948</v>
+      </c>
+      <c r="AQ159">
+        <f t="shared" si="22"/>
+        <v>20210.333333333332</v>
+      </c>
+      <c r="AR159">
+        <f t="shared" si="22"/>
+        <v>19583.5</v>
+      </c>
+      <c r="AS159">
+        <f t="shared" si="22"/>
+        <v>18916.833333333332</v>
+      </c>
+      <c r="AT159">
+        <f t="shared" si="22"/>
+        <v>17867</v>
+      </c>
+      <c r="AU159">
+        <f t="shared" si="22"/>
+        <v>17406.666666666668</v>
+      </c>
+      <c r="AV159">
+        <f t="shared" si="22"/>
+        <v>16626</v>
+      </c>
+      <c r="AW159">
+        <f t="shared" si="22"/>
+        <v>16196.666666666666</v>
+      </c>
+      <c r="AX159">
+        <f t="shared" si="22"/>
+        <v>15454.166666666666</v>
+      </c>
+      <c r="AY159">
+        <f t="shared" si="22"/>
+        <v>15104</v>
+      </c>
+      <c r="AZ159">
+        <f t="shared" si="22"/>
+        <v>14598.333333333334</v>
+      </c>
+    </row>
     <row r="161" spans="7:12" x14ac:dyDescent="0.4">
       <c r="G161" s="4" t="s">
         <v>158</v>
@@ -17194,11 +17409,11 @@
         <v>33825.666666666664</v>
       </c>
       <c r="I163">
-        <f t="shared" ref="I163:I183" si="22">H163-$H$164</f>
+        <f t="shared" ref="I163:I184" si="23">H163-$H$164</f>
         <v>5235.9999999999964</v>
       </c>
       <c r="J163">
-        <f t="shared" ref="J163:J183" si="23">I163/$I$162*100</f>
+        <f t="shared" ref="J163:J184" si="24">I163/$I$162*100</f>
         <v>26.677536047281791</v>
       </c>
       <c r="K163">
@@ -17206,7 +17421,7 @@
         <v>2054.1561122108842</v>
       </c>
       <c r="L163">
-        <f t="shared" ref="L163:L183" si="24">K163/H163*J163</f>
+        <f t="shared" ref="L163:L184" si="25">K163/H163*J163</f>
         <v>1.6200663321811866</v>
       </c>
     </row>
@@ -17218,11 +17433,11 @@
         <v>28589.666666666668</v>
       </c>
       <c r="I164">
-        <f t="shared" si="22"/>
+        <f t="shared" si="23"/>
         <v>0</v>
       </c>
       <c r="J164">
-        <f t="shared" si="23"/>
+        <f t="shared" si="24"/>
         <v>0</v>
       </c>
       <c r="K164">
@@ -17230,7 +17445,7 @@
         <v>1874.8243473278592</v>
       </c>
       <c r="L164">
-        <f t="shared" si="24"/>
+        <f t="shared" si="25"/>
         <v>0</v>
       </c>
     </row>
@@ -17242,11 +17457,11 @@
         <v>59694</v>
       </c>
       <c r="I165">
-        <f t="shared" si="22"/>
+        <f t="shared" si="23"/>
         <v>31104.333333333332</v>
       </c>
       <c r="J165">
-        <f t="shared" si="23"/>
+        <f t="shared" si="24"/>
         <v>158.47726770944789</v>
       </c>
       <c r="K165">
@@ -17254,7 +17469,7 @@
         <v>2695.2270776318642</v>
       </c>
       <c r="L165">
-        <f t="shared" si="24"/>
+        <f t="shared" si="25"/>
         <v>7.1553627352768752</v>
       </c>
     </row>
@@ -17266,11 +17481,11 @@
         <v>34945.333333333336</v>
       </c>
       <c r="I166">
-        <f t="shared" si="22"/>
+        <f t="shared" si="23"/>
         <v>6355.6666666666679</v>
       </c>
       <c r="J166">
-        <f t="shared" si="23"/>
+        <f t="shared" si="24"/>
         <v>32.382262529508679</v>
       </c>
       <c r="K166">
@@ -17278,7 +17493,7 @@
         <v>3823.969708736372</v>
       </c>
       <c r="L166">
-        <f t="shared" si="24"/>
+        <f t="shared" si="25"/>
         <v>3.543500067148404</v>
       </c>
     </row>
@@ -17290,11 +17505,11 @@
         <v>68141.333333333328</v>
       </c>
       <c r="I167">
-        <f t="shared" si="22"/>
+        <f t="shared" si="23"/>
         <v>39551.666666666657</v>
       </c>
       <c r="J167">
-        <f t="shared" si="23"/>
+        <f t="shared" si="24"/>
         <v>201.5166182639561</v>
       </c>
       <c r="K167">
@@ -17302,7 +17517,7 @@
         <v>1424.6670956168439</v>
       </c>
       <c r="L167">
-        <f t="shared" si="24"/>
+        <f t="shared" si="25"/>
         <v>4.213215110661741</v>
       </c>
     </row>
@@ -17314,11 +17529,11 @@
         <v>36085.666666666664</v>
       </c>
       <c r="I168">
-        <f t="shared" si="22"/>
+        <f t="shared" si="23"/>
         <v>7495.9999999999964</v>
       </c>
       <c r="J168">
-        <f t="shared" si="23"/>
+        <f t="shared" si="24"/>
         <v>38.192286136444679</v>
       </c>
       <c r="K168">
@@ -17326,7 +17541,7 @@
         <v>615.75671602779403</v>
       </c>
       <c r="L168">
-        <f t="shared" si="24"/>
+        <f t="shared" si="25"/>
         <v>0.65170353941928072</v>
       </c>
     </row>
@@ -17338,11 +17553,11 @@
         <v>37789.666666666664</v>
       </c>
       <c r="I169">
-        <f t="shared" si="22"/>
+        <f t="shared" si="23"/>
         <v>9199.9999999999964</v>
       </c>
       <c r="J169">
-        <f t="shared" si="23"/>
+        <f t="shared" si="24"/>
         <v>46.874203902786967</v>
       </c>
       <c r="K169">
@@ -17350,7 +17565,7 @@
         <v>1889.0689064545352</v>
       </c>
       <c r="L169">
-        <f t="shared" si="24"/>
+        <f t="shared" si="25"/>
         <v>2.343196141120536</v>
       </c>
     </row>
@@ -17362,11 +17577,11 @@
         <v>36471</v>
       </c>
       <c r="I170">
-        <f t="shared" si="22"/>
+        <f t="shared" si="23"/>
         <v>7881.3333333333321</v>
       </c>
       <c r="J170">
-        <f t="shared" si="23"/>
+        <f t="shared" si="24"/>
         <v>40.155568010054175</v>
       </c>
       <c r="K170">
@@ -17374,7 +17589,7 @@
         <v>1712.7883698811129</v>
       </c>
       <c r="L170">
-        <f t="shared" si="24"/>
+        <f t="shared" si="25"/>
         <v>1.885826817844064</v>
       </c>
     </row>
@@ -17386,11 +17601,11 @@
         <v>39563.666666666664</v>
       </c>
       <c r="I171">
-        <f t="shared" si="22"/>
+        <f t="shared" si="23"/>
         <v>10973.999999999996</v>
       </c>
       <c r="J171">
-        <f t="shared" si="23"/>
+        <f t="shared" si="24"/>
         <v>55.912773220563508</v>
       </c>
       <c r="K171">
@@ -17398,7 +17613,7 @@
         <v>733.15846399897293</v>
       </c>
       <c r="L171">
-        <f t="shared" si="24"/>
+        <f t="shared" si="25"/>
         <v>1.0361254753682567</v>
       </c>
     </row>
@@ -17410,11 +17625,11 @@
         <v>38954.333333333336</v>
       </c>
       <c r="I172">
-        <f t="shared" si="22"/>
+        <f t="shared" si="23"/>
         <v>10364.666666666668</v>
       </c>
       <c r="J172">
-        <f t="shared" si="23"/>
+        <f t="shared" si="24"/>
         <v>52.808206382364439</v>
       </c>
       <c r="K172">
@@ -17422,7 +17637,7 @@
         <v>616.87302853450592</v>
       </c>
       <c r="L172">
-        <f t="shared" si="24"/>
+        <f t="shared" si="25"/>
         <v>0.83626019020299946</v>
       </c>
     </row>
@@ -17434,11 +17649,11 @@
         <v>38425</v>
       </c>
       <c r="I173">
-        <f t="shared" si="22"/>
+        <f t="shared" si="23"/>
         <v>9835.3333333333321</v>
       </c>
       <c r="J173">
-        <f t="shared" si="23"/>
+        <f t="shared" si="24"/>
         <v>50.111241317233066</v>
       </c>
       <c r="K173">
@@ -17446,7 +17661,7 @@
         <v>1358.5400251740837</v>
       </c>
       <c r="L173">
-        <f t="shared" si="24"/>
+        <f t="shared" si="25"/>
         <v>1.7717144317662561</v>
       </c>
     </row>
@@ -17458,11 +17673,11 @@
         <v>48397</v>
       </c>
       <c r="I174">
-        <f t="shared" si="22"/>
+        <f t="shared" si="23"/>
         <v>19807.333333333332</v>
       </c>
       <c r="J174">
-        <f t="shared" si="23"/>
+        <f t="shared" si="24"/>
         <v>100.9188023301235</v>
       </c>
       <c r="K174">
@@ -17470,7 +17685,7 @@
         <v>3298.5384642292715</v>
       </c>
       <c r="L174">
-        <f t="shared" si="24"/>
+        <f t="shared" si="25"/>
         <v>6.8782063196037573</v>
       </c>
     </row>
@@ -17482,11 +17697,11 @@
         <v>61227.333333333336</v>
       </c>
       <c r="I175">
-        <f t="shared" si="22"/>
+        <f t="shared" si="23"/>
         <v>32637.666666666668</v>
       </c>
       <c r="J175">
-        <f t="shared" si="23"/>
+        <f t="shared" si="24"/>
         <v>166.28963502657908</v>
       </c>
       <c r="K175">
@@ -17494,7 +17709,7 @@
         <v>4744.0268057140374</v>
       </c>
       <c r="L175">
-        <f t="shared" si="24"/>
+        <f t="shared" si="25"/>
         <v>12.88448219333133</v>
       </c>
     </row>
@@ -17506,11 +17721,11 @@
         <v>39668.666666666664</v>
       </c>
       <c r="I176">
-        <f t="shared" si="22"/>
+        <f t="shared" si="23"/>
         <v>11078.999999999996</v>
       </c>
       <c r="J176">
-        <f t="shared" si="23"/>
+        <f t="shared" si="24"/>
         <v>56.447750547714868</v>
       </c>
       <c r="K176">
@@ -17518,7 +17733,7 @@
         <v>1331.2138570993518</v>
       </c>
       <c r="L176">
-        <f t="shared" si="24"/>
+        <f t="shared" si="25"/>
         <v>1.8942917432198096</v>
       </c>
     </row>
@@ -17530,11 +17745,11 @@
         <v>38096.666666666664</v>
       </c>
       <c r="I177">
-        <f t="shared" si="22"/>
+        <f t="shared" si="23"/>
         <v>9506.9999999999964</v>
       </c>
       <c r="J177">
-        <f t="shared" si="23"/>
+        <f t="shared" si="24"/>
         <v>48.438375706934316</v>
       </c>
       <c r="K177">
@@ -17542,7 +17757,7 @@
         <v>2536.0296396795788</v>
       </c>
       <c r="L177">
-        <f t="shared" si="24"/>
+        <f t="shared" si="25"/>
         <v>3.2244594406523941</v>
       </c>
     </row>
@@ -17554,11 +17769,11 @@
         <v>35698.666666666664</v>
       </c>
       <c r="I178">
-        <f t="shared" si="22"/>
+        <f t="shared" si="23"/>
         <v>7108.9999999999964</v>
       </c>
       <c r="J178">
-        <f t="shared" si="23"/>
+        <f t="shared" si="24"/>
         <v>36.220512559229626</v>
       </c>
       <c r="K178">
@@ -17566,7 +17781,7 @@
         <v>5225.6767344845639</v>
       </c>
       <c r="L178">
-        <f t="shared" si="24"/>
+        <f t="shared" si="25"/>
         <v>5.3020660844066692</v>
       </c>
     </row>
@@ -17578,11 +17793,11 @@
         <v>43964</v>
       </c>
       <c r="I179">
-        <f t="shared" si="22"/>
+        <f t="shared" si="23"/>
         <v>15374.333333333332</v>
       </c>
       <c r="J179">
-        <f t="shared" si="23"/>
+        <f t="shared" si="24"/>
         <v>78.332569080008838</v>
       </c>
       <c r="K179">
@@ -17590,7 +17805,7 @@
         <v>7141.9360820438596</v>
       </c>
       <c r="L179">
-        <f t="shared" si="24"/>
+        <f t="shared" si="25"/>
         <v>12.72509784168202</v>
       </c>
     </row>
@@ -17602,11 +17817,11 @@
         <v>40892.666666666664</v>
       </c>
       <c r="I180">
-        <f t="shared" si="22"/>
+        <f t="shared" si="23"/>
         <v>12302.999999999996</v>
       </c>
       <c r="J180">
-        <f t="shared" si="23"/>
+        <f t="shared" si="24"/>
         <v>62.684057675650884</v>
       </c>
       <c r="K180">
@@ -17614,7 +17829,7 @@
         <v>916.95492437378471</v>
       </c>
       <c r="L180">
-        <f t="shared" si="24"/>
+        <f t="shared" si="25"/>
         <v>1.4055932285842225</v>
       </c>
     </row>
@@ -17626,11 +17841,11 @@
         <v>39428.333333333336</v>
       </c>
       <c r="I181">
-        <f t="shared" si="22"/>
+        <f t="shared" si="23"/>
         <v>10838.666666666668</v>
       </c>
       <c r="J181">
-        <f t="shared" si="23"/>
+        <f t="shared" si="24"/>
         <v>55.223246887790644</v>
       </c>
       <c r="K181">
@@ -17638,7 +17853,7 @@
         <v>1766.7035216281574</v>
       </c>
       <c r="L181">
-        <f t="shared" si="24"/>
+        <f t="shared" si="25"/>
         <v>2.4744415120869316</v>
       </c>
     </row>
@@ -17650,11 +17865,11 @@
         <v>37468.666666666664</v>
       </c>
       <c r="I182">
-        <f t="shared" si="22"/>
+        <f t="shared" si="23"/>
         <v>8878.9999999999964</v>
       </c>
       <c r="J182">
-        <f t="shared" si="23"/>
+        <f t="shared" si="24"/>
         <v>45.23870178835277</v>
       </c>
       <c r="K182">
@@ -17662,7 +17877,7 @@
         <v>3335.5869548451788</v>
       </c>
       <c r="L182">
-        <f t="shared" si="24"/>
+        <f t="shared" si="25"/>
         <v>4.0273016619938646</v>
       </c>
     </row>
@@ -17674,11 +17889,11 @@
         <v>36237</v>
       </c>
       <c r="I183">
-        <f t="shared" si="22"/>
+        <f t="shared" si="23"/>
         <v>7647.3333333333321</v>
       </c>
       <c r="J183">
-        <f t="shared" si="23"/>
+        <f t="shared" si="24"/>
         <v>38.963332823831124</v>
       </c>
       <c r="K183">
@@ -17686,8 +17901,32 @@
         <v>1822.2532754806616</v>
       </c>
       <c r="L183">
+        <f t="shared" si="25"/>
+        <v>1.9593526191977659</v>
+      </c>
+    </row>
+    <row r="184" spans="7:12" x14ac:dyDescent="0.4">
+      <c r="G184" s="3" t="s">
+        <v>164</v>
+      </c>
+      <c r="H184">
+        <v>36897.666666666664</v>
+      </c>
+      <c r="I184">
+        <f t="shared" si="23"/>
+        <v>8307.9999999999964</v>
+      </c>
+      <c r="J184">
         <f t="shared" si="24"/>
-        <v>1.9593526191977659</v>
+        <v>42.329444133081964</v>
+      </c>
+      <c r="K184">
+        <f>STDEV(H72,H83,H84)</f>
+        <v>5363.1711079671186</v>
+      </c>
+      <c r="L184">
+        <f t="shared" si="25"/>
+        <v>6.1526939858216902</v>
       </c>
     </row>
   </sheetData>

</xml_diff>